<commit_message>
fixing no pembayaran pembelian
</commit_message>
<xml_diff>
--- a/PROGRESS MAKMUR PERMAI.xlsx
+++ b/PROGRESS MAKMUR PERMAI.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
   <si>
     <t>No.</t>
   </si>
@@ -309,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -400,6 +406,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +719,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -719,7 +731,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +805,7 @@
       <c r="F3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H3" s="15"/>
@@ -818,7 +830,7 @@
       <c r="F4" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H4" s="15"/>
@@ -843,7 +855,7 @@
       <c r="F5" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H5" s="15"/>
@@ -868,7 +880,7 @@
       <c r="F6" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="15"/>
@@ -893,7 +905,7 @@
       <c r="F7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H7" s="15"/>
@@ -918,7 +930,7 @@
       <c r="F8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H8" s="15"/>
@@ -943,7 +955,7 @@
       <c r="F9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="21" t="s">
         <v>78</v>
       </c>
       <c r="H9" s="15"/>
@@ -1014,10 +1026,16 @@
         <v>28</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="D13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>78</v>
+      </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="20" t="s">
+        <v>78</v>
+      </c>
       <c r="H13" s="15"/>
       <c r="I13" s="9"/>
     </row>

</xml_diff>